<commit_message>
working on analysis and presentation prep
</commit_message>
<xml_diff>
--- a/data/freezingexp.xlsx
+++ b/data/freezingexp.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9400" yWindow="2300" windowWidth="36680" windowHeight="22120" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="9980" yWindow="2540" windowWidth="36680" windowHeight="22120" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1997" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2019" uniqueCount="453">
   <si>
     <t>OLD</t>
   </si>
@@ -1392,6 +1392,12 @@
   </si>
   <si>
     <t>tx</t>
+  </si>
+  <si>
+    <t>23/3/17</t>
+  </si>
+  <si>
+    <t>27/3/17</t>
   </si>
 </sst>
 </file>
@@ -2077,7 +2083,7 @@
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A139" sqref="A139:XFD139"/>
+      <selection pane="bottomLeft" activeCell="S1" sqref="S1:T1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7771,10 +7777,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N149"/>
+  <dimension ref="A1:P149"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N38" sqref="N38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7783,7 +7789,7 @@
     <col min="9" max="9" width="10.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -7826,8 +7832,14 @@
       <c r="N1" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O1" t="s">
+        <v>451</v>
+      </c>
+      <c r="P1" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>93</v>
       </c>
@@ -7856,8 +7868,14 @@
       <c r="M2" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O2">
+        <v>11</v>
+      </c>
+      <c r="P2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -7883,8 +7901,14 @@
       <c r="M3" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O3">
+        <v>10</v>
+      </c>
+      <c r="P3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>90</v>
       </c>
@@ -7899,8 +7923,14 @@
       <c r="M4" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O4">
+        <v>9</v>
+      </c>
+      <c r="P4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>92</v>
       </c>
@@ -7923,8 +7953,14 @@
       <c r="M5" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O5">
+        <v>11</v>
+      </c>
+      <c r="P5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -7939,8 +7975,14 @@
       <c r="M6" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O6" s="16" t="s">
+        <v>437</v>
+      </c>
+      <c r="P6" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>88</v>
       </c>
@@ -7952,8 +7994,14 @@
       <c r="M7" s="13" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O7">
+        <v>9</v>
+      </c>
+      <c r="P7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>99</v>
       </c>
@@ -7973,8 +8021,14 @@
       <c r="M8" s="1" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O8">
+        <v>11</v>
+      </c>
+      <c r="P8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>120</v>
       </c>
@@ -7998,8 +8052,14 @@
       <c r="M9" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O9">
+        <v>12</v>
+      </c>
+      <c r="P9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>102</v>
       </c>
@@ -8021,7 +8081,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>105</v>
       </c>
@@ -8046,7 +8106,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>109</v>
       </c>
@@ -8071,7 +8131,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>108</v>
       </c>
@@ -8093,7 +8153,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>104</v>
       </c>
@@ -8106,7 +8166,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>112</v>
       </c>
@@ -8132,8 +8192,14 @@
       <c r="M15" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O15">
+        <v>10</v>
+      </c>
+      <c r="P15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -8143,8 +8209,14 @@
       <c r="E16" s="7"/>
       <c r="H16" s="1"/>
       <c r="M16" s="1"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O16">
+        <v>10</v>
+      </c>
+      <c r="P16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>126</v>
       </c>
@@ -8154,8 +8226,14 @@
       <c r="E17" s="7"/>
       <c r="H17" s="1"/>
       <c r="M17" s="1"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O17">
+        <v>10</v>
+      </c>
+      <c r="P17">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>130</v>
       </c>
@@ -8170,8 +8248,14 @@
       <c r="M18" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O18">
+        <v>3</v>
+      </c>
+      <c r="P18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>131</v>
       </c>
@@ -8195,8 +8279,14 @@
       <c r="M19" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O19">
+        <v>10</v>
+      </c>
+      <c r="P19">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>127</v>
       </c>
@@ -8214,8 +8304,14 @@
       </c>
       <c r="H20" s="1"/>
       <c r="M20" s="1"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O20">
+        <v>10</v>
+      </c>
+      <c r="P20">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>129</v>
       </c>
@@ -8228,8 +8324,14 @@
       </c>
       <c r="H21" s="1"/>
       <c r="M21" s="1"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O21">
+        <v>12</v>
+      </c>
+      <c r="P21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>148</v>
       </c>
@@ -8242,8 +8344,14 @@
       </c>
       <c r="H22" s="1"/>
       <c r="M22" s="1"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O22">
+        <v>11</v>
+      </c>
+      <c r="P22">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>141</v>
       </c>
@@ -8280,8 +8388,14 @@
       <c r="M23" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O23">
+        <v>2</v>
+      </c>
+      <c r="P23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>159</v>
       </c>
@@ -8293,8 +8407,14 @@
       <c r="M24" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O24">
+        <v>5</v>
+      </c>
+      <c r="P24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>94</v>
       </c>
@@ -8318,8 +8438,14 @@
       <c r="M25" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O25">
+        <v>4</v>
+      </c>
+      <c r="P25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>95</v>
       </c>
@@ -8346,8 +8472,14 @@
       <c r="N26">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O26">
+        <v>4</v>
+      </c>
+      <c r="P26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>96</v>
       </c>
@@ -8357,8 +8489,11 @@
       <c r="E27" s="7"/>
       <c r="H27" s="1"/>
       <c r="M27" s="1"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P27" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>97</v>
       </c>
@@ -8370,8 +8505,14 @@
       <c r="M28" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O28" t="s">
+        <v>437</v>
+      </c>
+      <c r="P28">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -8389,8 +8530,14 @@
       <c r="M29" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O29">
+        <v>4</v>
+      </c>
+      <c r="P29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>11</v>
       </c>
@@ -8405,8 +8552,14 @@
       <c r="M30" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O30">
+        <v>11</v>
+      </c>
+      <c r="P30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>89</v>
       </c>
@@ -8432,8 +8585,14 @@
       <c r="M31" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O31">
+        <v>4</v>
+      </c>
+      <c r="P31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>121</v>
       </c>
@@ -8448,8 +8607,14 @@
       <c r="N32">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O32">
+        <v>4</v>
+      </c>
+      <c r="P32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>122</v>
       </c>
@@ -8469,8 +8634,14 @@
       <c r="N33">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O33">
+        <v>3</v>
+      </c>
+      <c r="P33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>116</v>
       </c>
@@ -8488,8 +8659,11 @@
       <c r="M34" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P34">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>124</v>
       </c>
@@ -8499,8 +8673,14 @@
       <c r="E35" s="7"/>
       <c r="H35" s="1"/>
       <c r="M35" s="1"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O35">
+        <v>2</v>
+      </c>
+      <c r="P35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>209</v>
       </c>
@@ -8530,7 +8710,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>113</v>
       </c>
@@ -8548,8 +8728,11 @@
       <c r="N37">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P37">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>119</v>
       </c>
@@ -8561,8 +8744,11 @@
       <c r="M38" s="1" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P38">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>110</v>
       </c>
@@ -8591,8 +8777,14 @@
       <c r="M39" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O39">
+        <v>9</v>
+      </c>
+      <c r="P39">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>123</v>
       </c>
@@ -8618,8 +8810,14 @@
       <c r="M40" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O40">
+        <v>4</v>
+      </c>
+      <c r="P40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>115</v>
       </c>
@@ -8643,8 +8841,14 @@
       <c r="M41" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O41">
+        <v>5</v>
+      </c>
+      <c r="P41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>135</v>
       </c>
@@ -8657,8 +8861,14 @@
         <v>9</v>
       </c>
       <c r="M42" s="1"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O42">
+        <v>2</v>
+      </c>
+      <c r="P42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>137</v>
       </c>
@@ -8685,8 +8895,11 @@
       <c r="N43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P43">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>132</v>
       </c>
@@ -8699,8 +8912,14 @@
       <c r="E44" s="7"/>
       <c r="H44" s="1"/>
       <c r="M44" s="1"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O44">
+        <v>5</v>
+      </c>
+      <c r="P44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>136</v>
       </c>
@@ -8713,8 +8932,14 @@
       <c r="E45" s="7"/>
       <c r="H45" s="1"/>
       <c r="M45" s="1"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O45">
+        <v>12</v>
+      </c>
+      <c r="P45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>133</v>
       </c>
@@ -8730,8 +8955,14 @@
         <v>9</v>
       </c>
       <c r="M46" s="1"/>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O46">
+        <v>12</v>
+      </c>
+      <c r="P46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>134</v>
       </c>
@@ -8741,8 +8972,14 @@
       <c r="E47" s="7"/>
       <c r="H47" s="1"/>
       <c r="M47" s="1"/>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O47">
+        <v>4</v>
+      </c>
+      <c r="P47">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>150</v>
       </c>
@@ -8768,8 +9005,14 @@
       <c r="M48" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O48">
+        <v>4</v>
+      </c>
+      <c r="P48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>152</v>
       </c>
@@ -8801,8 +9044,14 @@
       <c r="M49" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O49">
+        <v>4</v>
+      </c>
+      <c r="P49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>157</v>
       </c>
@@ -8831,8 +9080,14 @@
       <c r="M50" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O50">
+        <v>5</v>
+      </c>
+      <c r="P50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>160</v>
       </c>
@@ -8842,8 +9097,14 @@
       <c r="E51" s="7"/>
       <c r="H51" s="1"/>
       <c r="M51" s="1"/>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O51">
+        <v>4</v>
+      </c>
+      <c r="P51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>172</v>
       </c>
@@ -8875,8 +9136,14 @@
       <c r="M52" s="1" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O52">
+        <v>4</v>
+      </c>
+      <c r="P52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>167</v>
       </c>
@@ -8906,7 +9173,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>4</v>
       </c>
@@ -8926,8 +9193,14 @@
       <c r="M54">
         <v>11</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O54">
+        <v>2</v>
+      </c>
+      <c r="P54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>25</v>
       </c>
@@ -8942,7 +9215,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>13</v>
       </c>
@@ -8962,8 +9235,11 @@
       <c r="N56">
         <v>3</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P56">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>20</v>
       </c>
@@ -8989,7 +9265,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>29</v>
       </c>
@@ -9010,7 +9286,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>17</v>
       </c>
@@ -9031,7 +9307,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>15</v>
       </c>
@@ -9063,7 +9339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>18</v>
       </c>
@@ -9092,7 +9368,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>30</v>
       </c>
@@ -9120,8 +9396,14 @@
       <c r="M62">
         <v>2</v>
       </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O62">
+        <v>13</v>
+      </c>
+      <c r="P62" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>24</v>
       </c>
@@ -9147,7 +9429,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>26</v>
       </c>
@@ -9172,8 +9454,14 @@
       <c r="M64">
         <v>5</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O64">
+        <v>14</v>
+      </c>
+      <c r="P64" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>27</v>
       </c>
@@ -9195,8 +9483,14 @@
       <c r="M65">
         <v>4</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O65">
+        <v>13</v>
+      </c>
+      <c r="P65" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>32</v>
       </c>
@@ -9209,8 +9503,14 @@
       <c r="I66" s="6">
         <v>9</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O66">
+        <v>13</v>
+      </c>
+      <c r="P66" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>40</v>
       </c>
@@ -9232,8 +9532,14 @@
       <c r="M67">
         <v>2</v>
       </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O67">
+        <v>14</v>
+      </c>
+      <c r="P67" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
         <v>42</v>
       </c>
@@ -9250,8 +9556,11 @@
       <c r="N68">
         <v>2</v>
       </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O68" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>34</v>
       </c>
@@ -9259,8 +9568,11 @@
         <v>5</v>
       </c>
       <c r="I69" s="6"/>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O69" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>35</v>
       </c>
@@ -9269,7 +9581,7 @@
       </c>
       <c r="I70" s="6"/>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>38</v>
       </c>
@@ -9278,7 +9590,7 @@
       </c>
       <c r="I71" s="6"/>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>53</v>
       </c>
@@ -9287,7 +9599,7 @@
       </c>
       <c r="I72" s="6"/>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>51</v>
       </c>
@@ -9295,8 +9607,14 @@
         <v>5</v>
       </c>
       <c r="I73" s="6"/>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O73">
+        <v>13</v>
+      </c>
+      <c r="P73" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>56</v>
       </c>
@@ -9307,8 +9625,14 @@
         <v>9</v>
       </c>
       <c r="I74" s="6"/>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O74">
+        <v>14</v>
+      </c>
+      <c r="P74" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>64</v>
       </c>
@@ -9340,7 +9664,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>86</v>
       </c>
@@ -9370,7 +9694,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>101</v>
       </c>
@@ -9398,7 +9722,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>107</v>
       </c>
@@ -9428,7 +9752,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>114</v>
       </c>
@@ -9453,7 +9777,7 @@
       </c>
       <c r="M79" s="1"/>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>106</v>
       </c>
@@ -9904,7 +10228,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>178</v>
       </c>
@@ -9933,7 +10257,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>71</v>
       </c>
@@ -9959,7 +10283,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>81</v>
       </c>
@@ -9988,7 +10312,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>183</v>
       </c>
@@ -10009,7 +10333,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>184</v>
       </c>
@@ -10036,7 +10360,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>75</v>
       </c>
@@ -10062,7 +10386,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>80</v>
       </c>
@@ -10088,7 +10412,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>222</v>
       </c>
@@ -10114,7 +10438,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>180</v>
       </c>
@@ -10138,7 +10462,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>77</v>
       </c>
@@ -10164,7 +10488,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>173</v>
       </c>
@@ -10190,7 +10514,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>176</v>
       </c>
@@ -10219,7 +10543,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>191</v>
       </c>
@@ -10245,7 +10569,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A110" s="4" t="s">
         <v>117</v>
       </c>
@@ -10272,7 +10596,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
         <v>118</v>
       </c>
@@ -10298,8 +10622,11 @@
       <c r="M111" s="1" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O111" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A112" s="4" t="s">
         <v>151</v>
       </c>
@@ -10329,6 +10656,12 @@
         <v>376</v>
       </c>
       <c r="M112" s="1"/>
+      <c r="O112">
+        <v>4</v>
+      </c>
+      <c r="P112" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A113" s="4" t="s">
@@ -10789,7 +11122,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A129" s="4" t="s">
         <v>82</v>
       </c>
@@ -10818,7 +11151,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A130" s="4" t="s">
         <v>196</v>
       </c>
@@ -10845,7 +11178,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A131" s="4" t="s">
         <v>72</v>
       </c>
@@ -10869,7 +11202,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A132" s="4" t="s">
         <v>197</v>
       </c>
@@ -10893,7 +11226,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A133" s="4" t="s">
         <v>189</v>
       </c>
@@ -10927,7 +11260,7 @@
       </c>
       <c r="M133" s="1"/>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A134" s="4" t="s">
         <v>194</v>
       </c>
@@ -10959,8 +11292,14 @@
         <v>368</v>
       </c>
       <c r="M134" s="1"/>
-    </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O134">
+        <v>2</v>
+      </c>
+      <c r="P134" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="135" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A135" s="4" t="s">
         <v>175</v>
       </c>
@@ -10993,8 +11332,14 @@
         <v>368</v>
       </c>
       <c r="M135" s="1"/>
-    </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O135">
+        <v>3</v>
+      </c>
+      <c r="P135" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="136" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A136" s="4" t="s">
         <v>186</v>
       </c>
@@ -11021,8 +11366,14 @@
         <v>368</v>
       </c>
       <c r="M136" s="1"/>
-    </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O136">
+        <v>4</v>
+      </c>
+      <c r="P136" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="137" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A137" s="4" t="s">
         <v>84</v>
       </c>
@@ -11054,8 +11405,14 @@
       <c r="M137" s="1" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O137">
+        <v>1</v>
+      </c>
+      <c r="P137" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="138" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A138" s="4" t="s">
         <v>69</v>
       </c>
@@ -11089,7 +11446,7 @@
       </c>
       <c r="M138" s="1"/>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A139" s="4" t="s">
         <v>22</v>
       </c>
@@ -11114,8 +11471,14 @@
       <c r="L139" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O139">
+        <v>2</v>
+      </c>
+      <c r="P139" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="140" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A140" s="4" t="s">
         <v>50</v>
       </c>
@@ -11141,7 +11504,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A141" s="4" t="s">
         <v>44</v>
       </c>
@@ -11158,7 +11521,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A142" s="4" t="s">
         <v>54</v>
       </c>
@@ -11190,7 +11553,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A143" s="4" t="s">
         <v>46</v>
       </c>
@@ -11225,7 +11588,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A144" s="4" t="s">
         <v>47</v>
       </c>
@@ -11390,7 +11753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+    <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated data sheets for recording
</commit_message>
<xml_diff>
--- a/data/freezingexp.xlsx
+++ b/data/freezingexp.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2029" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2073" uniqueCount="463">
   <si>
     <t>OLD</t>
   </si>
@@ -1413,6 +1413,21 @@
   </si>
   <si>
     <t>post.scale</t>
+  </si>
+  <si>
+    <t>BBCH 04.4</t>
+  </si>
+  <si>
+    <t>BBCH 07.4</t>
+  </si>
+  <si>
+    <t>BBCH 10.7</t>
+  </si>
+  <si>
+    <t>04.APR</t>
+  </si>
+  <si>
+    <t>05.APR</t>
   </si>
 </sst>
 </file>
@@ -2095,23 +2110,26 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V149"/>
+  <dimension ref="A1:AA149"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U1" sqref="U1"/>
+    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="V27" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="V36" sqref="V36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="12" width="10.83203125" customWidth="1"/>
+    <col min="3" max="12" width="10.83203125" customWidth="1"/>
     <col min="13" max="13" width="10.83203125" style="1" customWidth="1"/>
-    <col min="14" max="17" width="10.83203125" customWidth="1"/>
+    <col min="14" max="22" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2176,10 +2194,25 @@
         <v>453</v>
       </c>
       <c r="V1" t="s">
+        <v>458</v>
+      </c>
+      <c r="W1" t="s">
+        <v>459</v>
+      </c>
+      <c r="X1" t="s">
+        <v>460</v>
+      </c>
+      <c r="Y1" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="Z1" t="s">
+        <v>211</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2226,8 +2259,11 @@
       <c r="U2">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="V2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2260,8 +2296,11 @@
       <c r="U3">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="V3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2302,8 +2341,11 @@
       <c r="U4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="V4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2339,8 +2381,14 @@
       <c r="U5">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="V5">
+        <v>14</v>
+      </c>
+      <c r="W5" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -2370,8 +2418,11 @@
       <c r="U6" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="V6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>98</v>
       </c>
@@ -2409,8 +2460,11 @@
       <c r="U7">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="V7" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2452,8 +2506,11 @@
       <c r="U8">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="V8" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>103</v>
       </c>
@@ -2484,7 +2541,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -2503,8 +2560,11 @@
       <c r="I10" s="7"/>
       <c r="L10" s="1"/>
       <c r="Q10" s="1"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>125</v>
       </c>
@@ -2524,7 +2584,7 @@
       <c r="L11" s="1"/>
       <c r="Q11" s="1"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -2552,7 +2612,7 @@
       <c r="L12" s="1"/>
       <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -2575,7 +2635,7 @@
       <c r="L13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -2598,7 +2658,7 @@
       <c r="L14" s="1"/>
       <c r="Q14" s="1"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -2653,8 +2713,11 @@
       <c r="U15">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="V15" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>158</v>
       </c>
@@ -2685,7 +2748,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -2727,8 +2790,11 @@
       <c r="U17">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V17">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>6</v>
       </c>
@@ -2774,7 +2840,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -2802,8 +2868,11 @@
       <c r="U19">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V19">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -2833,8 +2902,11 @@
       <c r="U20">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V20">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -2874,7 +2946,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -2911,7 +2983,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>3</v>
       </c>
@@ -2958,8 +3030,11 @@
       <c r="U23">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V23" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>21</v>
       </c>
@@ -2993,7 +3068,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>21</v>
       </c>
@@ -3029,7 +3104,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>12</v>
       </c>
@@ -3066,7 +3141,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -3089,7 +3164,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -3137,7 +3212,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>100</v>
       </c>
@@ -3174,7 +3249,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -3205,7 +3280,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>14</v>
       </c>
@@ -3253,7 +3328,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>14</v>
       </c>
@@ -3298,7 +3373,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>23</v>
       </c>
@@ -3341,7 +3416,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -3372,8 +3447,14 @@
       <c r="U34">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V34">
+        <v>9</v>
+      </c>
+      <c r="W34">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>41</v>
       </c>
@@ -3415,8 +3496,11 @@
       <c r="U35">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V35" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>125</v>
       </c>
@@ -3439,7 +3523,7 @@
       <c r="L36" s="1"/>
       <c r="Q36" s="1"/>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>125</v>
       </c>
@@ -3467,8 +3551,11 @@
       <c r="U37">
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V37">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -3499,8 +3586,11 @@
       <c r="U38">
         <v>9</v>
       </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V38">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -3528,8 +3618,11 @@
       <c r="U39">
         <v>10</v>
       </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V39">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>149</v>
       </c>
@@ -3574,7 +3667,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>144</v>
       </c>
@@ -3625,7 +3718,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>144</v>
       </c>
@@ -3673,7 +3766,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>158</v>
       </c>
@@ -3698,8 +3791,11 @@
       <c r="U43">
         <v>9</v>
       </c>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V43">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>171</v>
       </c>
@@ -3750,7 +3846,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>3</v>
       </c>
@@ -3794,8 +3890,11 @@
       <c r="U45">
         <v>3</v>
       </c>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V45" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>21</v>
       </c>
@@ -3831,7 +3930,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>12</v>
       </c>
@@ -3873,7 +3972,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>19</v>
       </c>
@@ -3923,7 +4022,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>28</v>
       </c>
@@ -3962,7 +4061,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>16</v>
       </c>
@@ -4001,7 +4100,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>14</v>
       </c>
@@ -4051,7 +4150,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>23</v>
       </c>
@@ -4098,7 +4197,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>23</v>
       </c>
@@ -4142,7 +4241,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>31</v>
       </c>
@@ -4167,8 +4266,14 @@
       <c r="M54" s="6">
         <v>9</v>
       </c>
-    </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V54">
+        <v>9</v>
+      </c>
+      <c r="W54">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>41</v>
       </c>
@@ -4204,7 +4309,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>33</v>
       </c>
@@ -4224,8 +4329,11 @@
         <v>8.4</v>
       </c>
       <c r="M56" s="6"/>
-    </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W56">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>37</v>
       </c>
@@ -4252,7 +4360,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>36</v>
       </c>
@@ -4272,8 +4380,11 @@
         <v>9.6</v>
       </c>
       <c r="M58" s="6"/>
-    </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V58">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>52</v>
       </c>
@@ -4294,7 +4405,7 @@
       </c>
       <c r="M59" s="6"/>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>49</v>
       </c>
@@ -4315,7 +4426,7 @@
       </c>
       <c r="M60" s="6"/>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>55</v>
       </c>
@@ -4338,8 +4449,11 @@
         <v>9</v>
       </c>
       <c r="M61" s="6"/>
-    </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W61">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>63</v>
       </c>
@@ -4386,7 +4500,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>6</v>
       </c>
@@ -4431,7 +4545,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>6</v>
       </c>
@@ -4473,7 +4587,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>14</v>
       </c>
@@ -4510,7 +4624,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>111</v>
       </c>
@@ -4552,7 +4666,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>14</v>
       </c>
@@ -4592,7 +4706,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>23</v>
       </c>
@@ -4629,7 +4743,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>19</v>
       </c>
@@ -4666,7 +4780,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>100</v>
       </c>
@@ -4706,7 +4820,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>21</v>
       </c>
@@ -4748,7 +4862,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>19</v>
       </c>
@@ -4785,7 +4899,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>100</v>
       </c>
@@ -4822,7 +4936,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>125</v>
       </c>
@@ -4853,7 +4967,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>33</v>
       </c>
@@ -4893,7 +5007,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>52</v>
       </c>
@@ -4938,7 +5052,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>43</v>
       </c>
@@ -4975,7 +5089,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>139</v>
       </c>
@@ -5011,7 +5125,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>144</v>
       </c>
@@ -5044,7 +5158,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>43</v>
       </c>
@@ -5080,7 +5194,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>142</v>
       </c>
@@ -5119,7 +5233,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>59</v>
       </c>
@@ -5158,7 +5272,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>162</v>
       </c>
@@ -5196,7 +5310,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>162</v>
       </c>
@@ -5234,7 +5348,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>61</v>
       </c>
@@ -5272,7 +5386,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>61</v>
       </c>
@@ -5318,7 +5432,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>57</v>
       </c>
@@ -5361,7 +5475,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>73</v>
       </c>
@@ -5404,7 +5518,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>170</v>
       </c>
@@ -5440,7 +5554,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>78</v>
       </c>
@@ -5479,7 +5593,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>70</v>
       </c>
@@ -5520,7 +5634,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>177</v>
       </c>
@@ -5561,7 +5675,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>70</v>
       </c>
@@ -5602,7 +5716,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>70</v>
       </c>
@@ -5646,7 +5760,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>177</v>
       </c>
@@ -5679,7 +5793,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>177</v>
       </c>
@@ -5718,7 +5832,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>73</v>
       </c>
@@ -5759,7 +5873,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>73</v>
       </c>
@@ -5800,7 +5914,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>73</v>
       </c>
@@ -5841,7 +5955,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>76</v>
       </c>
@@ -5877,7 +5991,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>76</v>
       </c>
@@ -5918,7 +6032,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>66</v>
       </c>
@@ -5956,7 +6070,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>66</v>
       </c>
@@ -5997,7 +6111,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>66</v>
       </c>
@@ -6035,7 +6149,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="4" t="s">
         <v>23</v>
       </c>
@@ -6074,7 +6188,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
         <v>14</v>
       </c>
@@ -6113,7 +6227,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="4" t="s">
         <v>43</v>
       </c>
@@ -6156,7 +6270,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="4" t="s">
         <v>43</v>
       </c>
@@ -6199,7 +6313,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="4" t="s">
         <v>43</v>
       </c>
@@ -6239,7 +6353,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="4" t="s">
         <v>142</v>
       </c>
@@ -6290,7 +6404,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
         <v>142</v>
       </c>
@@ -6331,7 +6445,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="4" t="s">
         <v>57</v>
       </c>
@@ -6379,7 +6493,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="4" t="s">
         <v>61</v>
       </c>
@@ -6424,7 +6538,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="4" t="s">
         <v>61</v>
       </c>
@@ -6462,7 +6576,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="9" t="s">
         <v>61</v>
       </c>
@@ -6501,7 +6615,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="4" t="s">
         <v>61</v>
       </c>
@@ -6554,7 +6668,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="4" t="s">
         <v>170</v>
       </c>
@@ -6595,7 +6709,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="4" t="s">
         <v>78</v>
       </c>
@@ -6634,7 +6748,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="4" t="s">
         <v>70</v>
       </c>
@@ -6670,7 +6784,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="4" t="s">
         <v>67</v>
       </c>
@@ -6712,7 +6826,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="4" t="s">
         <v>177</v>
       </c>
@@ -6751,7 +6865,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="4" t="s">
         <v>177</v>
       </c>
@@ -6787,7 +6901,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="4" t="s">
         <v>73</v>
       </c>
@@ -6823,7 +6937,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="4" t="s">
         <v>73</v>
       </c>
@@ -6864,7 +6978,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="4" t="s">
         <v>73</v>
       </c>
@@ -6908,7 +7022,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="4" t="s">
         <v>195</v>
       </c>
@@ -6947,7 +7061,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="4" t="s">
         <v>66</v>
       </c>
@@ -6986,7 +7100,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="4" t="s">
         <v>195</v>
       </c>
@@ -7022,7 +7136,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="129" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="4" t="s">
         <v>78</v>
       </c>
@@ -7068,7 +7182,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="130" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="4" t="s">
         <v>70</v>
       </c>
@@ -7113,7 +7227,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="131" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="4" t="s">
         <v>67</v>
       </c>
@@ -7159,7 +7273,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="132" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="4" t="s">
         <v>73</v>
       </c>
@@ -7199,7 +7313,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="133" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="4" t="s">
         <v>83</v>
       </c>
@@ -7247,7 +7361,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="134" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="4" t="s">
         <v>66</v>
       </c>
@@ -7296,7 +7410,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="135" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="4" t="s">
         <v>14</v>
       </c>
@@ -7343,7 +7457,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="136" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="4" t="s">
         <v>23</v>
       </c>
@@ -7387,7 +7501,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="137" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="4" t="s">
         <v>14</v>
       </c>
@@ -7437,7 +7551,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="138" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="4" t="s">
         <v>21</v>
       </c>
@@ -7478,7 +7592,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="139" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="4" t="s">
         <v>39</v>
       </c>
@@ -7519,7 +7633,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="140" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="4" t="s">
         <v>49</v>
       </c>
@@ -7560,7 +7674,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="141" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="4" t="s">
         <v>43</v>
       </c>
@@ -7592,7 +7706,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="142" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="4" t="s">
         <v>43</v>
       </c>
@@ -7639,7 +7753,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="143" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="4" t="s">
         <v>45</v>
       </c>
@@ -7689,7 +7803,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="144" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="4" t="s">
         <v>43</v>
       </c>
@@ -7730,7 +7844,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="145" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="4" t="s">
         <v>43</v>
       </c>
@@ -7774,7 +7888,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="146" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="4" t="s">
         <v>78</v>
       </c>
@@ -7812,7 +7926,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="147" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="4" t="s">
         <v>78</v>
       </c>
@@ -7853,7 +7967,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="148" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="4" t="s">
         <v>78</v>
       </c>
@@ -7888,7 +8002,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="149" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="4" t="s">
         <v>78</v>
       </c>
@@ -7928,7 +8042,7 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="34" fitToHeight="4" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup scale="29" fitToHeight="2" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -11937,10 +12051,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O71"/>
+  <dimension ref="A1:O79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O44" sqref="O44"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="I77" sqref="I77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13837,6 +13951,214 @@
         <v>91</v>
       </c>
       <c r="H71" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>133</v>
+      </c>
+      <c r="B72" t="s">
+        <v>461</v>
+      </c>
+      <c r="C72" s="3">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="E72" s="3">
+        <v>0.26805555555555555</v>
+      </c>
+      <c r="F72">
+        <v>12</v>
+      </c>
+      <c r="G72" t="s">
+        <v>91</v>
+      </c>
+      <c r="H72" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>97</v>
+      </c>
+      <c r="B73" t="s">
+        <v>461</v>
+      </c>
+      <c r="C73" s="3">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="E73" s="3">
+        <v>0.26805555555555555</v>
+      </c>
+      <c r="F73">
+        <v>12</v>
+      </c>
+      <c r="G73" t="s">
+        <v>91</v>
+      </c>
+      <c r="H73" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>38</v>
+      </c>
+      <c r="B74" t="s">
+        <v>461</v>
+      </c>
+      <c r="C74" s="3">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="E74" s="3">
+        <v>0.26805555555555555</v>
+      </c>
+      <c r="F74">
+        <v>11</v>
+      </c>
+      <c r="G74" t="s">
+        <v>5</v>
+      </c>
+      <c r="H74" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>94</v>
+      </c>
+      <c r="B75" t="s">
+        <v>461</v>
+      </c>
+      <c r="C75" s="3">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="E75" s="3">
+        <v>0.26805555555555555</v>
+      </c>
+      <c r="F75">
+        <v>13</v>
+      </c>
+      <c r="G75" t="s">
+        <v>91</v>
+      </c>
+      <c r="H75" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>134</v>
+      </c>
+      <c r="B76" t="s">
+        <v>461</v>
+      </c>
+      <c r="C76" s="3">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="E76" s="3">
+        <v>0.26805555555555555</v>
+      </c>
+      <c r="F76">
+        <v>14</v>
+      </c>
+      <c r="G76" t="s">
+        <v>91</v>
+      </c>
+      <c r="H76" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>136</v>
+      </c>
+      <c r="B77" t="s">
+        <v>461</v>
+      </c>
+      <c r="C77" s="3">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="E77" s="3">
+        <v>0.26805555555555555</v>
+      </c>
+      <c r="F77">
+        <v>13</v>
+      </c>
+      <c r="G77" t="s">
+        <v>91</v>
+      </c>
+      <c r="H77" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>160</v>
+      </c>
+      <c r="B78" t="s">
+        <v>461</v>
+      </c>
+      <c r="C78" s="3">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="E78" s="3">
+        <v>0.26805555555555555</v>
+      </c>
+      <c r="F78">
+        <v>13</v>
+      </c>
+      <c r="G78" t="s">
+        <v>91</v>
+      </c>
+      <c r="H78" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>96</v>
+      </c>
+      <c r="B79" t="s">
+        <v>461</v>
+      </c>
+      <c r="C79" s="3">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="E79" s="3">
+        <v>0.26805555555555555</v>
+      </c>
+      <c r="F79">
+        <v>11</v>
+      </c>
+      <c r="G79" t="s">
+        <v>91</v>
+      </c>
+      <c r="H79" s="8">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating figures and analysis
</commit_message>
<xml_diff>
--- a/data/freezingexp.xlsx
+++ b/data/freezingexp.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="1200" windowWidth="42440" windowHeight="21640" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="3780" yWindow="1200" windowWidth="42440" windowHeight="21640" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2102" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2115" uniqueCount="470">
   <si>
     <t>OLD</t>
   </si>
@@ -1430,9 +1430,6 @@
     <t>BBCH 10.4</t>
   </si>
   <si>
-    <t>07.APR</t>
-  </si>
-  <si>
     <t>Data can be found on FRZ sheet</t>
   </si>
   <si>
@@ -1440,6 +1437,18 @@
   </si>
   <si>
     <t>11.APR</t>
+  </si>
+  <si>
+    <t>10.APR</t>
+  </si>
+  <si>
+    <t>17.APR</t>
+  </si>
+  <si>
+    <t>BBCH 17.4</t>
+  </si>
+  <si>
+    <t>BBCH 15.4</t>
   </si>
 </sst>
 </file>
@@ -2113,7 +2122,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
   </sheetData>
@@ -2127,14 +2136,14 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA149"/>
+  <dimension ref="A1:AB149"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="P34" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="Y2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="Y57" sqref="Y57"/>
+      <selection pane="bottomRight" activeCell="AA49" sqref="AA49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2146,7 +2155,7 @@
     <col min="14" max="22" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2220,16 +2229,19 @@
         <v>462</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="Z1" t="s">
+        <v>464</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>468</v>
+      </c>
+      <c r="AB1" t="s">
         <v>211</v>
       </c>
-      <c r="AA1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2280,7 +2292,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2320,7 +2332,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2365,7 +2377,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2408,7 +2420,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -2442,7 +2454,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>98</v>
       </c>
@@ -2484,7 +2496,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2530,7 +2542,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>103</v>
       </c>
@@ -2561,7 +2573,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -2586,8 +2598,11 @@
       <c r="Y10">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA10" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>125</v>
       </c>
@@ -2606,8 +2621,14 @@
       <c r="I11" s="7"/>
       <c r="L11" s="1"/>
       <c r="Q11" s="1"/>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="Z11">
+        <v>9</v>
+      </c>
+      <c r="AA11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -2635,7 +2656,7 @@
       <c r="L12" s="1"/>
       <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -2658,7 +2679,7 @@
       <c r="L13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -2681,7 +2702,7 @@
       <c r="L14" s="1"/>
       <c r="Q14" s="1"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -2740,7 +2761,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>158</v>
       </c>
@@ -2771,7 +2792,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -2820,7 +2841,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>6</v>
       </c>
@@ -2869,7 +2890,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -2900,8 +2921,11 @@
       <c r="V19">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA19" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -2938,7 +2962,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -2978,7 +3002,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -3018,7 +3042,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>3</v>
       </c>
@@ -3069,7 +3093,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>21</v>
       </c>
@@ -3103,7 +3127,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>21</v>
       </c>
@@ -3142,7 +3166,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>12</v>
       </c>
@@ -3179,7 +3203,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -3202,7 +3226,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -3250,7 +3274,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>100</v>
       </c>
@@ -3287,7 +3311,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -3318,7 +3342,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>14</v>
       </c>
@@ -3366,7 +3390,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>14</v>
       </c>
@@ -3411,7 +3435,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>23</v>
       </c>
@@ -3454,7 +3478,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -3492,7 +3516,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>41</v>
       </c>
@@ -3538,7 +3562,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>125</v>
       </c>
@@ -3561,7 +3585,7 @@
       <c r="L36" s="1"/>
       <c r="Q36" s="1"/>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>125</v>
       </c>
@@ -3592,8 +3616,11 @@
       <c r="V37">
         <v>13</v>
       </c>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA37" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -3628,7 +3655,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -3660,7 +3687,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>149</v>
       </c>
@@ -3708,7 +3735,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>144</v>
       </c>
@@ -3762,7 +3789,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>144</v>
       </c>
@@ -3810,7 +3837,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>158</v>
       </c>
@@ -3839,7 +3866,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>171</v>
       </c>
@@ -3890,7 +3917,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>3</v>
       </c>
@@ -3938,7 +3965,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>21</v>
       </c>
@@ -3973,8 +4000,11 @@
       <c r="U46">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA46" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>12</v>
       </c>
@@ -4015,8 +4045,11 @@
       <c r="U47">
         <v>4</v>
       </c>
-    </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA47" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>19</v>
       </c>
@@ -4064,6 +4097,9 @@
       </c>
       <c r="U48">
         <v>3</v>
+      </c>
+      <c r="AA48" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.2">
@@ -12104,10 +12140,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O82"/>
+  <dimension ref="A1:O84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H83" sqref="H83"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13981,13 +14017,13 @@
         <v>2</v>
       </c>
       <c r="I70" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="J70" s="3">
         <v>0.40069444444444446</v>
       </c>
       <c r="K70" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="L70" s="3">
         <v>0.43333333333333335</v>
@@ -14103,13 +14139,13 @@
         <v>2</v>
       </c>
       <c r="I74" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="J74" s="3">
         <v>0.40069444444444446</v>
       </c>
       <c r="K74" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="L74" s="3">
         <v>0.43333333333333335</v>
@@ -14256,13 +14292,13 @@
         <v>135</v>
       </c>
       <c r="B80" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="C80" s="3">
         <v>0.40069444444444446</v>
       </c>
       <c r="D80" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E80" s="3">
         <v>0.43333333333333335</v>
@@ -14282,13 +14318,13 @@
         <v>32</v>
       </c>
       <c r="B81" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="C81" s="3">
         <v>0.40069444444444446</v>
       </c>
       <c r="D81" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E81" s="3">
         <v>0.43333333333333335</v>
@@ -14308,13 +14344,13 @@
         <v>56</v>
       </c>
       <c r="B82" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="C82" s="3">
         <v>0.40069444444444446</v>
       </c>
       <c r="D82" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E82" s="3">
         <v>0.43333333333333335</v>
@@ -14327,6 +14363,40 @@
       </c>
       <c r="H82" s="8">
         <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>132</v>
+      </c>
+      <c r="B83" t="s">
+        <v>467</v>
+      </c>
+      <c r="C83" s="3">
+        <v>0.3576388888888889</v>
+      </c>
+      <c r="F83">
+        <v>13</v>
+      </c>
+      <c r="G83" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>34</v>
+      </c>
+      <c r="B84" t="s">
+        <v>467</v>
+      </c>
+      <c r="C84" s="3">
+        <v>0.3576388888888889</v>
+      </c>
+      <c r="F84">
+        <v>13</v>
+      </c>
+      <c r="G84" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finally cleaned all data
</commit_message>
<xml_diff>
--- a/data/freezingexp.xlsx
+++ b/data/freezingexp.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="1200" windowWidth="42440" windowHeight="21640" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3780" yWindow="1200" windowWidth="42440" windowHeight="21640" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2128" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2130" uniqueCount="473">
   <si>
     <t>OLD</t>
   </si>
@@ -1455,6 +1455,9 @@
   </si>
   <si>
     <t>BBCH 24.4</t>
+  </si>
+  <si>
+    <t>18.APR</t>
   </si>
 </sst>
 </file>
@@ -2144,12 +2147,12 @@
   </sheetPr>
   <dimension ref="A1:AC149"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="E97" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="AC59" sqref="AC59"/>
+      <selection pane="bottomRight" activeCell="X37" sqref="X37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3617,6 +3620,9 @@
       <c r="I36" s="7"/>
       <c r="L36" s="1"/>
       <c r="Q36" s="1"/>
+      <c r="X36">
+        <v>9</v>
+      </c>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
@@ -12187,8 +12193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O84"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="I74" sqref="I74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14420,11 +14426,20 @@
       <c r="C83" s="3">
         <v>0.3576388888888889</v>
       </c>
+      <c r="D83" t="s">
+        <v>472</v>
+      </c>
+      <c r="E83" s="3">
+        <v>0.3298611111111111</v>
+      </c>
       <c r="F83">
         <v>13</v>
       </c>
       <c r="G83" t="s">
         <v>91</v>
+      </c>
+      <c r="H83" s="8">
+        <v>3</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
@@ -14437,11 +14452,20 @@
       <c r="C84" s="3">
         <v>0.3576388888888889</v>
       </c>
+      <c r="D84" t="s">
+        <v>472</v>
+      </c>
+      <c r="E84" s="3">
+        <v>0.3298611111111111</v>
+      </c>
       <c r="F84">
         <v>13</v>
       </c>
       <c r="G84" t="s">
         <v>5</v>
+      </c>
+      <c r="H84" s="8">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>